<commit_message>
feat: import baby carers
</commit_message>
<xml_diff>
--- a/public/static/template/import_baby.xlsx
+++ b/public/static/template/import_baby.xlsx
@@ -16,7 +16,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
-    <t>宝宝id</t>
+    <r>
+      <t>宝宝</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue (Headings)"/>
+        <charset val="134"/>
+      </rPr>
+      <t>id</t>
+    </r>
   </si>
   <si>
     <t>成长阶段</t>
@@ -52,52 +64,52 @@
     <t>CHW_ID</t>
   </si>
   <si>
-    <t>Caregiver I_name*main</t>
+    <t>Caregiver_Main_name</t>
   </si>
   <si>
-    <t>Caregiver I_relationship*main</t>
+    <t>Caregiver_Main_relationship</t>
   </si>
   <si>
-    <t>Caregiver I_phone main</t>
+    <t>Caregiver_Main_phone</t>
   </si>
   <si>
-    <t>Caregiver I_Wechat</t>
+    <t>Caregiver_Main_Wechat</t>
   </si>
   <si>
-    <t>Caregiver II_name</t>
+    <t>Caregiver_II_name</t>
   </si>
   <si>
-    <t>Caregiver II_relationship</t>
+    <t>Caregiver_II_relationship</t>
   </si>
   <si>
-    <t>Caregiver II_phone</t>
+    <t>Caregiver_II_phone</t>
   </si>
   <si>
-    <t>Caregiver II_Wechat</t>
+    <t>Caregiver_II_Wechat</t>
   </si>
   <si>
-    <t>Caregiver III_name</t>
+    <t>Caregiver_III_name</t>
   </si>
   <si>
-    <t>Caregiver III_relationship</t>
+    <t>Caregiver_III_relationship</t>
   </si>
   <si>
-    <t>Caregiver III_phone</t>
+    <t>Caregiver_III_phone</t>
   </si>
   <si>
-    <t>Caregiver III_Wechat</t>
+    <t>Caregiver_III_Wechat</t>
   </si>
   <si>
-    <t>Caregiver IV_name</t>
+    <t>Caregiver_IV_name</t>
   </si>
   <si>
-    <t>Caregiver IV_relationship</t>
+    <t>Caregiver_IV_relationship</t>
   </si>
   <si>
-    <t>Caregiver IV_phone</t>
+    <t>Caregiver_IV_phone</t>
   </si>
   <si>
-    <t>Caregiver IV_Wechat</t>
+    <t>Caregiver_IV_Wechat</t>
   </si>
   <si>
     <t>1.必填
@@ -212,7 +224,7 @@
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -230,7 +242,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Helvetica Neue (Headings)"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
@@ -249,10 +261,12 @@
       <scheme val="major"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="等线"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
       <charset val="134"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
@@ -263,17 +277,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -285,7 +298,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,78 +335,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -398,12 +365,66 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue (Headings)"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="35">
@@ -427,13 +448,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -445,13 +502,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,43 +520,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -517,24 +538,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -547,37 +550,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,7 +574,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -607,7 +628,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -636,24 +657,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -670,6 +673,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -680,21 +707,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,16 +745,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -751,10 +772,10 @@
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -763,121 +784,121 @@
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -898,10 +919,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -919,16 +940,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2105,10 +2126,10 @@
   <sheetPr/>
   <dimension ref="A1:AC196"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="T1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.75" customHeight="1"/>
@@ -2159,7 +2180,7 @@
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="7" t="s">

</xml_diff>

<commit_message>
fix: update imprt babies templates
</commit_message>
<xml_diff>
--- a/public/static/template/import_baby.xlsx
+++ b/public/static/template/import_baby.xlsx
@@ -184,10 +184,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -219,23 +219,8 @@
       <scheme val="major"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,13 +234,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -263,7 +241,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -271,9 +249,31 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -286,25 +286,18 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -333,8 +326,30 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -343,21 +358,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -398,7 +398,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,25 +464,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,121 +494,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -572,13 +518,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -607,16 +607,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -637,15 +637,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -661,17 +652,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -681,6 +666,30 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -695,61 +704,55 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -758,97 +761,94 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1029,8 +1029,8 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="00F2607A"/>
       <color rgb="00EBABB5"/>
-      <color rgb="00F2607A"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2085,7 +2085,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.75" customHeight="1"/>
@@ -2157,16 +2157,16 @@
       <c r="K1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="15" t="s">
@@ -2242,16 +2242,16 @@
         <v>37</v>
       </c>
       <c r="K2" s="16"/>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="7" t="s">
         <v>41</v>
       </c>
       <c r="P2" s="17" t="s">
@@ -8287,20 +8287,20 @@
     </row>
   </sheetData>
   <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B196">
+      <formula1>"待产期,已出生"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D196">
       <formula1>"男,女,未知"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B196">
-      <formula1>"待产期,已出生"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N196">
-      <formula1>"母亲,父亲,(外)祖母,(外)祖父,亲姐妹,亲兄弟,其他"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G196">
+      <formula1>"已添加,未添加"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H196">
       <formula1>"纯母乳喂养,纯奶粉喂养,母乳奶粉混合喂养,已终止母乳/奶粉喂养"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G196">
-      <formula1>"已添加,未添加"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N196">
+      <formula1>"母亲,父亲,(外)祖母,(外)祖父,亲姐妹,亲兄弟,其他"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: update import babies template
</commit_message>
<xml_diff>
--- a/public/static/template/import_baby.xlsx
+++ b/public/static/template/import_baby.xlsx
@@ -161,7 +161,7 @@
     <t>1.必填</t>
   </si>
   <si>
-    <t>1.校验：表格内不重复；2.chw必须存在;</t>
+    <t>1.chw必须存在;</t>
   </si>
   <si>
     <t>1. 必填
@@ -184,10 +184,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -219,10 +219,33 @@
       <scheme val="major"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -233,8 +256,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -249,21 +288,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,33 +318,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -322,21 +330,6 @@
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -370,6 +363,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,7 +398,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,49 +410,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,7 +446,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,103 +560,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -607,17 +607,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -638,6 +632,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -648,24 +666,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -707,148 +707,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2082,10 +2082,10 @@
   <sheetPr/>
   <dimension ref="A1:AC196"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.75" customHeight="1"/>

</xml_diff>

<commit_message>
fix: update import babies templete
</commit_message>
<xml_diff>
--- a/public/static/template/import_baby.xlsx
+++ b/public/static/template/import_baby.xlsx
@@ -184,9 +184,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
@@ -219,11 +219,17 @@
       <scheme val="major"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -234,31 +240,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,17 +270,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -318,8 +293,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -334,15 +333,23 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -358,13 +365,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -398,13 +398,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,103 +530,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -530,7 +548,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,43 +572,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -607,15 +607,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -631,17 +622,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -649,8 +634,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -688,8 +673,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -707,152 +707,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -899,8 +899,14 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2085,7 +2091,7 @@
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.75" customHeight="1"/>
@@ -2157,7 +2163,7 @@
       <c r="K1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="15" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="12" t="s">
@@ -2169,7 +2175,7 @@
       <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="P1" s="16" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="14" t="s">
@@ -2241,8 +2247,8 @@
       <c r="J2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="7" t="s">
+      <c r="K2" s="17"/>
+      <c r="L2" s="18" t="s">
         <v>38</v>
       </c>
       <c r="M2" s="7" t="s">
@@ -2254,22 +2260,22 @@
       <c r="O2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="16"/>
-      <c r="AC2" s="16"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
     </row>
     <row r="3" s="3" customFormat="1" ht="35" customHeight="1" spans="1:29">
       <c r="A3" s="8"/>
@@ -2280,7 +2286,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
-      <c r="I3" s="18"/>
+      <c r="I3" s="20"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="8"/>
@@ -2311,7 +2317,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
-      <c r="I4" s="18"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
@@ -8296,11 +8302,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G196">
       <formula1>"已添加,未添加"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N196">
+      <formula1>"母亲,父亲,(外)祖母,(外)祖父,亲姐妹,亲兄弟,其他"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H196">
       <formula1>"纯母乳喂养,纯奶粉喂养,母乳奶粉混合喂养,已终止母乳/奶粉喂养"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N196">
-      <formula1>"母亲,父亲,(外)祖母,(外)祖父,亲姐妹,亲兄弟,其他"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[HF-28][Zhen Tang]feat: update the upload template validation description
</commit_message>
<xml_diff>
--- a/public/static/template/import_baby.xlsx
+++ b/public/static/template/import_baby.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ztang/workspace/unc/src/visit-link-admin-web/public/static/template/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0319C8-35FF-6940-8989-72238FFDC093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9564"/>
+    <workbookView xWindow="8060" yWindow="10100" windowWidth="22360" windowHeight="9560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baby Roster" sheetId="1" r:id="rId1"/>
@@ -128,10 +134,6 @@
   </si>
   <si>
     <t>1.必填
-2.校验：2-10个汉字</t>
-  </si>
-  <si>
-    <t>1.必填
 2.选项：男/女/未知</t>
   </si>
   <si>
@@ -165,31 +167,29 @@
   </si>
   <si>
     <t>1. 必填
-2. 主看护人姓名:2-10个汉字</t>
+2. 亲属关系选项:爸爸/妈妈/爷爷/外公/奶奶/外婆/其他</t>
+  </si>
+  <si>
+    <t>主看护人微信</t>
   </si>
   <si>
     <t>1. 必填
-2. 亲属关系选项:爸爸/妈妈/爷爷/外公/奶奶/外婆/其他</t>
+2. 主看护人姓名:1-50个字符</t>
   </si>
   <si>
     <t>1. 必填
-2. 主看护人电话:11位手机号码</t>
+2. 主看护人电话: 5-20数字号码</t>
   </si>
   <si>
-    <t>主看护人微信</t>
+    <t>1.必填
+2.校验：1-50个字符，不包含特殊字符</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -200,7 +200,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
@@ -215,159 +215,8 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -377,7 +226,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,194 +245,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -606,267 +269,25 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -881,16 +302,16 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -908,61 +329,14 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
@@ -1032,13 +406,16 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
-      <color rgb="00F2607A"/>
-      <color rgb="00EBABB5"/>
+      <color rgb="FFF2607A"/>
+      <color rgb="FFEBABB5"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2077,55 +1454,54 @@
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC196"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Y1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.8333333333333" style="4" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="20" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.6666666666667" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.1666666666667" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.6666666666667" style="5" customWidth="1"/>
-    <col min="6" max="7" width="22.1666666666667" style="5" customWidth="1"/>
-    <col min="8" max="8" width="27.4444444444444" style="5" customWidth="1"/>
-    <col min="9" max="9" width="35.3333333333333" style="4" customWidth="1"/>
-    <col min="10" max="10" width="21.1666666666667" style="4" customWidth="1"/>
-    <col min="11" max="11" width="11.8333333333333" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" style="5" customWidth="1"/>
+    <col min="6" max="7" width="22.1640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="27.5" style="5" customWidth="1"/>
+    <col min="9" max="9" width="35.33203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.1640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" style="4" customWidth="1"/>
     <col min="12" max="12" width="14" style="4" customWidth="1"/>
-    <col min="13" max="13" width="22.3333333333333" style="4" customWidth="1"/>
-    <col min="14" max="14" width="25.3333333333333" style="4" customWidth="1"/>
-    <col min="15" max="15" width="23.6666666666667" style="4" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="23.6640625" style="4" customWidth="1"/>
     <col min="16" max="16" width="20" style="4" customWidth="1"/>
-    <col min="17" max="17" width="18.6666666666667" style="4" customWidth="1"/>
-    <col min="18" max="18" width="21.8333333333333" style="4" customWidth="1"/>
-    <col min="19" max="19" width="21.1666666666667" style="4" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="21.83203125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="21.1640625" style="4" customWidth="1"/>
     <col min="20" max="20" width="19.5" style="4" customWidth="1"/>
-    <col min="21" max="21" width="17.3333333333333" style="4" customWidth="1"/>
-    <col min="22" max="22" width="23.3333333333333" style="4" customWidth="1"/>
-    <col min="23" max="23" width="18.8333333333333" style="4" customWidth="1"/>
-    <col min="24" max="24" width="22.8333333333333" style="4" customWidth="1"/>
-    <col min="25" max="25" width="16.3333333333333" style="4" customWidth="1"/>
-    <col min="26" max="26" width="22.8333333333333" style="4" customWidth="1"/>
-    <col min="27" max="27" width="18.8333333333333" style="4" customWidth="1"/>
-    <col min="28" max="28" width="23.6666666666667" style="4" customWidth="1"/>
-    <col min="29" max="29" width="20.6666666666667" style="4" customWidth="1"/>
+    <col min="21" max="21" width="17.33203125" style="4" customWidth="1"/>
+    <col min="22" max="22" width="23.33203125" style="4" customWidth="1"/>
+    <col min="23" max="23" width="18.83203125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="22.83203125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="16.33203125" style="4" customWidth="1"/>
+    <col min="26" max="26" width="22.83203125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="18.83203125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="23.6640625" style="4" customWidth="1"/>
+    <col min="29" max="29" width="20.6640625" style="4" customWidth="1"/>
     <col min="30" max="30" width="9" style="4" customWidth="1"/>
     <col min="31" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="27.6" spans="1:29">
+    <row r="1" spans="1:29" s="1" customFormat="1" ht="30">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2212,7 +1588,7 @@
       </c>
       <c r="AC1" s="16"/>
     </row>
-    <row r="2" s="2" customFormat="1" ht="88" customHeight="1" spans="1:29">
+    <row r="2" spans="1:29" s="2" customFormat="1" ht="88" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>28</v>
       </c>
@@ -2220,44 +1596,44 @@
         <v>29</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="K2" s="18"/>
       <c r="L2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O2" s="8" t="s">
         <v>41</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
@@ -2273,7 +1649,7 @@
       <c r="AB2" s="18"/>
       <c r="AC2" s="18"/>
     </row>
-    <row r="3" s="3" customFormat="1" ht="35" customHeight="1" spans="1:29">
+    <row r="3" spans="1:29" s="3" customFormat="1" ht="35" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -2304,7 +1680,7 @@
       <c r="AB3" s="13"/>
       <c r="AC3" s="13"/>
     </row>
-    <row r="4" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="4" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -2335,7 +1711,7 @@
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
     </row>
-    <row r="5" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="5" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -2366,7 +1742,7 @@
       <c r="AB5" s="13"/>
       <c r="AC5" s="13"/>
     </row>
-    <row r="6" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="6" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -2397,7 +1773,7 @@
       <c r="AB6" s="13"/>
       <c r="AC6" s="13"/>
     </row>
-    <row r="7" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="7" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -2428,7 +1804,7 @@
       <c r="AB7" s="13"/>
       <c r="AC7" s="13"/>
     </row>
-    <row r="8" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="8" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -2459,7 +1835,7 @@
       <c r="AB8" s="13"/>
       <c r="AC8" s="13"/>
     </row>
-    <row r="9" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="9" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -2490,7 +1866,7 @@
       <c r="AB9" s="13"/>
       <c r="AC9" s="13"/>
     </row>
-    <row r="10" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="10" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -2521,7 +1897,7 @@
       <c r="AB10" s="13"/>
       <c r="AC10" s="13"/>
     </row>
-    <row r="11" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="11" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -2552,7 +1928,7 @@
       <c r="AB11" s="13"/>
       <c r="AC11" s="13"/>
     </row>
-    <row r="12" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="12" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -2583,7 +1959,7 @@
       <c r="AB12" s="13"/>
       <c r="AC12" s="13"/>
     </row>
-    <row r="13" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="13" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -2614,7 +1990,7 @@
       <c r="AB13" s="13"/>
       <c r="AC13" s="13"/>
     </row>
-    <row r="14" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="14" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -2645,7 +2021,7 @@
       <c r="AB14" s="13"/>
       <c r="AC14" s="13"/>
     </row>
-    <row r="15" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="15" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -2676,7 +2052,7 @@
       <c r="AB15" s="13"/>
       <c r="AC15" s="13"/>
     </row>
-    <row r="16" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="16" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -2707,7 +2083,7 @@
       <c r="AB16" s="13"/>
       <c r="AC16" s="13"/>
     </row>
-    <row r="17" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="17" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -2738,7 +2114,7 @@
       <c r="AB17" s="13"/>
       <c r="AC17" s="13"/>
     </row>
-    <row r="18" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="18" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -2769,7 +2145,7 @@
       <c r="AB18" s="13"/>
       <c r="AC18" s="13"/>
     </row>
-    <row r="19" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="19" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -2800,7 +2176,7 @@
       <c r="AB19" s="13"/>
       <c r="AC19" s="13"/>
     </row>
-    <row r="20" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="20" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -2831,7 +2207,7 @@
       <c r="AB20" s="13"/>
       <c r="AC20" s="13"/>
     </row>
-    <row r="21" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="21" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -2862,7 +2238,7 @@
       <c r="AB21" s="13"/>
       <c r="AC21" s="13"/>
     </row>
-    <row r="22" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="22" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -2893,7 +2269,7 @@
       <c r="AB22" s="13"/>
       <c r="AC22" s="13"/>
     </row>
-    <row r="23" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="23" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -2924,7 +2300,7 @@
       <c r="AB23" s="13"/>
       <c r="AC23" s="13"/>
     </row>
-    <row r="24" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="24" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -2955,7 +2331,7 @@
       <c r="AB24" s="13"/>
       <c r="AC24" s="13"/>
     </row>
-    <row r="25" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="25" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -2986,7 +2362,7 @@
       <c r="AB25" s="13"/>
       <c r="AC25" s="13"/>
     </row>
-    <row r="26" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="26" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -3017,7 +2393,7 @@
       <c r="AB26" s="13"/>
       <c r="AC26" s="13"/>
     </row>
-    <row r="27" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="27" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -3048,7 +2424,7 @@
       <c r="AB27" s="13"/>
       <c r="AC27" s="13"/>
     </row>
-    <row r="28" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="28" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -3079,7 +2455,7 @@
       <c r="AB28" s="13"/>
       <c r="AC28" s="13"/>
     </row>
-    <row r="29" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="29" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -3110,7 +2486,7 @@
       <c r="AB29" s="13"/>
       <c r="AC29" s="13"/>
     </row>
-    <row r="30" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="30" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -3141,7 +2517,7 @@
       <c r="AB30" s="13"/>
       <c r="AC30" s="13"/>
     </row>
-    <row r="31" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="31" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -3172,7 +2548,7 @@
       <c r="AB31" s="13"/>
       <c r="AC31" s="13"/>
     </row>
-    <row r="32" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="32" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -3203,7 +2579,7 @@
       <c r="AB32" s="13"/>
       <c r="AC32" s="13"/>
     </row>
-    <row r="33" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="33" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -3234,7 +2610,7 @@
       <c r="AB33" s="13"/>
       <c r="AC33" s="13"/>
     </row>
-    <row r="34" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="34" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -3265,7 +2641,7 @@
       <c r="AB34" s="13"/>
       <c r="AC34" s="13"/>
     </row>
-    <row r="35" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="35" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -3296,7 +2672,7 @@
       <c r="AB35" s="13"/>
       <c r="AC35" s="13"/>
     </row>
-    <row r="36" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="36" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -3327,7 +2703,7 @@
       <c r="AB36" s="13"/>
       <c r="AC36" s="13"/>
     </row>
-    <row r="37" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="37" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -3358,7 +2734,7 @@
       <c r="AB37" s="13"/>
       <c r="AC37" s="13"/>
     </row>
-    <row r="38" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="38" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -3389,7 +2765,7 @@
       <c r="AB38" s="13"/>
       <c r="AC38" s="13"/>
     </row>
-    <row r="39" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="39" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -3420,7 +2796,7 @@
       <c r="AB39" s="13"/>
       <c r="AC39" s="13"/>
     </row>
-    <row r="40" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="40" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -3451,7 +2827,7 @@
       <c r="AB40" s="13"/>
       <c r="AC40" s="13"/>
     </row>
-    <row r="41" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="41" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -3482,7 +2858,7 @@
       <c r="AB41" s="13"/>
       <c r="AC41" s="13"/>
     </row>
-    <row r="42" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="42" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -3513,7 +2889,7 @@
       <c r="AB42" s="13"/>
       <c r="AC42" s="13"/>
     </row>
-    <row r="43" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="43" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -3544,7 +2920,7 @@
       <c r="AB43" s="13"/>
       <c r="AC43" s="13"/>
     </row>
-    <row r="44" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="44" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -3575,7 +2951,7 @@
       <c r="AB44" s="13"/>
       <c r="AC44" s="13"/>
     </row>
-    <row r="45" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="45" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
@@ -3606,7 +2982,7 @@
       <c r="AB45" s="13"/>
       <c r="AC45" s="13"/>
     </row>
-    <row r="46" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="46" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
@@ -3637,7 +3013,7 @@
       <c r="AB46" s="13"/>
       <c r="AC46" s="13"/>
     </row>
-    <row r="47" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="47" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -3668,7 +3044,7 @@
       <c r="AB47" s="13"/>
       <c r="AC47" s="13"/>
     </row>
-    <row r="48" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="48" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
@@ -3699,7 +3075,7 @@
       <c r="AB48" s="13"/>
       <c r="AC48" s="13"/>
     </row>
-    <row r="49" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="49" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
@@ -3730,7 +3106,7 @@
       <c r="AB49" s="13"/>
       <c r="AC49" s="13"/>
     </row>
-    <row r="50" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="50" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
@@ -3761,7 +3137,7 @@
       <c r="AB50" s="13"/>
       <c r="AC50" s="13"/>
     </row>
-    <row r="51" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="51" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
@@ -3792,7 +3168,7 @@
       <c r="AB51" s="13"/>
       <c r="AC51" s="13"/>
     </row>
-    <row r="52" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="52" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
@@ -3823,7 +3199,7 @@
       <c r="AB52" s="13"/>
       <c r="AC52" s="13"/>
     </row>
-    <row r="53" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="53" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
@@ -3854,7 +3230,7 @@
       <c r="AB53" s="13"/>
       <c r="AC53" s="13"/>
     </row>
-    <row r="54" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="54" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
@@ -3885,7 +3261,7 @@
       <c r="AB54" s="13"/>
       <c r="AC54" s="13"/>
     </row>
-    <row r="55" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="55" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
@@ -3916,7 +3292,7 @@
       <c r="AB55" s="13"/>
       <c r="AC55" s="13"/>
     </row>
-    <row r="56" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="56" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
@@ -3947,7 +3323,7 @@
       <c r="AB56" s="13"/>
       <c r="AC56" s="13"/>
     </row>
-    <row r="57" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="57" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
@@ -3978,7 +3354,7 @@
       <c r="AB57" s="13"/>
       <c r="AC57" s="13"/>
     </row>
-    <row r="58" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="58" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
@@ -4009,7 +3385,7 @@
       <c r="AB58" s="13"/>
       <c r="AC58" s="13"/>
     </row>
-    <row r="59" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="59" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
@@ -4040,7 +3416,7 @@
       <c r="AB59" s="13"/>
       <c r="AC59" s="13"/>
     </row>
-    <row r="60" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="60" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
@@ -4071,7 +3447,7 @@
       <c r="AB60" s="13"/>
       <c r="AC60" s="13"/>
     </row>
-    <row r="61" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="61" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
@@ -4102,7 +3478,7 @@
       <c r="AB61" s="13"/>
       <c r="AC61" s="13"/>
     </row>
-    <row r="62" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="62" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -4133,7 +3509,7 @@
       <c r="AB62" s="13"/>
       <c r="AC62" s="13"/>
     </row>
-    <row r="63" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="63" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
@@ -4164,7 +3540,7 @@
       <c r="AB63" s="13"/>
       <c r="AC63" s="13"/>
     </row>
-    <row r="64" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="64" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
@@ -4195,7 +3571,7 @@
       <c r="AB64" s="13"/>
       <c r="AC64" s="13"/>
     </row>
-    <row r="65" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="65" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
@@ -4226,7 +3602,7 @@
       <c r="AB65" s="13"/>
       <c r="AC65" s="13"/>
     </row>
-    <row r="66" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="66" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="C66" s="13"/>
@@ -4257,7 +3633,7 @@
       <c r="AB66" s="13"/>
       <c r="AC66" s="13"/>
     </row>
-    <row r="67" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="67" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
@@ -4288,7 +3664,7 @@
       <c r="AB67" s="13"/>
       <c r="AC67" s="13"/>
     </row>
-    <row r="68" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="68" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
@@ -4319,7 +3695,7 @@
       <c r="AB68" s="13"/>
       <c r="AC68" s="13"/>
     </row>
-    <row r="69" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="69" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
@@ -4350,7 +3726,7 @@
       <c r="AB69" s="13"/>
       <c r="AC69" s="13"/>
     </row>
-    <row r="70" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="70" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13"/>
@@ -4381,7 +3757,7 @@
       <c r="AB70" s="13"/>
       <c r="AC70" s="13"/>
     </row>
-    <row r="71" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="71" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="13"/>
@@ -4412,7 +3788,7 @@
       <c r="AB71" s="13"/>
       <c r="AC71" s="13"/>
     </row>
-    <row r="72" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="72" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
@@ -4443,7 +3819,7 @@
       <c r="AB72" s="13"/>
       <c r="AC72" s="13"/>
     </row>
-    <row r="73" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="73" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
@@ -4474,7 +3850,7 @@
       <c r="AB73" s="13"/>
       <c r="AC73" s="13"/>
     </row>
-    <row r="74" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="74" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
@@ -4505,7 +3881,7 @@
       <c r="AB74" s="13"/>
       <c r="AC74" s="13"/>
     </row>
-    <row r="75" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="75" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
@@ -4536,7 +3912,7 @@
       <c r="AB75" s="13"/>
       <c r="AC75" s="13"/>
     </row>
-    <row r="76" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="76" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
@@ -4567,7 +3943,7 @@
       <c r="AB76" s="13"/>
       <c r="AC76" s="13"/>
     </row>
-    <row r="77" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="77" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
@@ -4598,7 +3974,7 @@
       <c r="AB77" s="13"/>
       <c r="AC77" s="13"/>
     </row>
-    <row r="78" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="78" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
@@ -4629,7 +4005,7 @@
       <c r="AB78" s="13"/>
       <c r="AC78" s="13"/>
     </row>
-    <row r="79" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="79" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
@@ -4660,7 +4036,7 @@
       <c r="AB79" s="13"/>
       <c r="AC79" s="13"/>
     </row>
-    <row r="80" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="80" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
@@ -4691,7 +4067,7 @@
       <c r="AB80" s="13"/>
       <c r="AC80" s="13"/>
     </row>
-    <row r="81" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="81" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
@@ -4722,7 +4098,7 @@
       <c r="AB81" s="13"/>
       <c r="AC81" s="13"/>
     </row>
-    <row r="82" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="82" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
@@ -4753,7 +4129,7 @@
       <c r="AB82" s="13"/>
       <c r="AC82" s="13"/>
     </row>
-    <row r="83" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="83" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
@@ -4784,7 +4160,7 @@
       <c r="AB83" s="13"/>
       <c r="AC83" s="13"/>
     </row>
-    <row r="84" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="84" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
@@ -4815,7 +4191,7 @@
       <c r="AB84" s="13"/>
       <c r="AC84" s="13"/>
     </row>
-    <row r="85" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="85" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
@@ -4846,7 +4222,7 @@
       <c r="AB85" s="13"/>
       <c r="AC85" s="13"/>
     </row>
-    <row r="86" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="86" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
@@ -4877,7 +4253,7 @@
       <c r="AB86" s="13"/>
       <c r="AC86" s="13"/>
     </row>
-    <row r="87" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="87" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A87" s="13"/>
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
@@ -4908,7 +4284,7 @@
       <c r="AB87" s="13"/>
       <c r="AC87" s="13"/>
     </row>
-    <row r="88" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="88" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A88" s="13"/>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -4939,7 +4315,7 @@
       <c r="AB88" s="13"/>
       <c r="AC88" s="13"/>
     </row>
-    <row r="89" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="89" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
@@ -4970,7 +4346,7 @@
       <c r="AB89" s="13"/>
       <c r="AC89" s="13"/>
     </row>
-    <row r="90" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="90" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
@@ -5001,7 +4377,7 @@
       <c r="AB90" s="13"/>
       <c r="AC90" s="13"/>
     </row>
-    <row r="91" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="91" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
@@ -5032,7 +4408,7 @@
       <c r="AB91" s="13"/>
       <c r="AC91" s="13"/>
     </row>
-    <row r="92" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="92" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
       <c r="C92" s="13"/>
@@ -5063,7 +4439,7 @@
       <c r="AB92" s="13"/>
       <c r="AC92" s="13"/>
     </row>
-    <row r="93" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="93" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="C93" s="13"/>
@@ -5094,7 +4470,7 @@
       <c r="AB93" s="13"/>
       <c r="AC93" s="13"/>
     </row>
-    <row r="94" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="94" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="C94" s="13"/>
@@ -5125,7 +4501,7 @@
       <c r="AB94" s="13"/>
       <c r="AC94" s="13"/>
     </row>
-    <row r="95" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="95" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A95" s="13"/>
       <c r="B95" s="13"/>
       <c r="C95" s="13"/>
@@ -5156,7 +4532,7 @@
       <c r="AB95" s="13"/>
       <c r="AC95" s="13"/>
     </row>
-    <row r="96" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="96" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A96" s="13"/>
       <c r="B96" s="13"/>
       <c r="C96" s="13"/>
@@ -5187,7 +4563,7 @@
       <c r="AB96" s="13"/>
       <c r="AC96" s="13"/>
     </row>
-    <row r="97" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="97" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A97" s="13"/>
       <c r="B97" s="13"/>
       <c r="C97" s="13"/>
@@ -5218,7 +4594,7 @@
       <c r="AB97" s="13"/>
       <c r="AC97" s="13"/>
     </row>
-    <row r="98" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="98" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A98" s="13"/>
       <c r="B98" s="13"/>
       <c r="C98" s="13"/>
@@ -5249,7 +4625,7 @@
       <c r="AB98" s="13"/>
       <c r="AC98" s="13"/>
     </row>
-    <row r="99" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="99" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A99" s="13"/>
       <c r="B99" s="13"/>
       <c r="C99" s="13"/>
@@ -5280,7 +4656,7 @@
       <c r="AB99" s="13"/>
       <c r="AC99" s="13"/>
     </row>
-    <row r="100" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="100" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A100" s="13"/>
       <c r="B100" s="13"/>
       <c r="C100" s="13"/>
@@ -5311,7 +4687,7 @@
       <c r="AB100" s="13"/>
       <c r="AC100" s="13"/>
     </row>
-    <row r="101" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="101" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A101" s="13"/>
       <c r="B101" s="13"/>
       <c r="C101" s="13"/>
@@ -5342,7 +4718,7 @@
       <c r="AB101" s="13"/>
       <c r="AC101" s="13"/>
     </row>
-    <row r="102" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="102" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A102" s="13"/>
       <c r="B102" s="13"/>
       <c r="C102" s="13"/>
@@ -5373,7 +4749,7 @@
       <c r="AB102" s="13"/>
       <c r="AC102" s="13"/>
     </row>
-    <row r="103" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="103" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A103" s="13"/>
       <c r="B103" s="13"/>
       <c r="C103" s="13"/>
@@ -5404,7 +4780,7 @@
       <c r="AB103" s="13"/>
       <c r="AC103" s="13"/>
     </row>
-    <row r="104" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="104" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A104" s="13"/>
       <c r="B104" s="13"/>
       <c r="C104" s="13"/>
@@ -5435,7 +4811,7 @@
       <c r="AB104" s="13"/>
       <c r="AC104" s="13"/>
     </row>
-    <row r="105" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="105" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A105" s="13"/>
       <c r="B105" s="13"/>
       <c r="C105" s="13"/>
@@ -5466,7 +4842,7 @@
       <c r="AB105" s="13"/>
       <c r="AC105" s="13"/>
     </row>
-    <row r="106" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="106" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
       <c r="C106" s="13"/>
@@ -5497,7 +4873,7 @@
       <c r="AB106" s="13"/>
       <c r="AC106" s="13"/>
     </row>
-    <row r="107" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="107" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A107" s="13"/>
       <c r="B107" s="13"/>
       <c r="C107" s="13"/>
@@ -5528,7 +4904,7 @@
       <c r="AB107" s="13"/>
       <c r="AC107" s="13"/>
     </row>
-    <row r="108" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="108" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A108" s="13"/>
       <c r="B108" s="13"/>
       <c r="C108" s="13"/>
@@ -5559,7 +4935,7 @@
       <c r="AB108" s="13"/>
       <c r="AC108" s="13"/>
     </row>
-    <row r="109" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="109" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A109" s="13"/>
       <c r="B109" s="13"/>
       <c r="C109" s="13"/>
@@ -5590,7 +4966,7 @@
       <c r="AB109" s="13"/>
       <c r="AC109" s="13"/>
     </row>
-    <row r="110" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="110" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A110" s="13"/>
       <c r="B110" s="13"/>
       <c r="C110" s="13"/>
@@ -5621,7 +4997,7 @@
       <c r="AB110" s="13"/>
       <c r="AC110" s="13"/>
     </row>
-    <row r="111" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="111" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A111" s="13"/>
       <c r="B111" s="13"/>
       <c r="C111" s="13"/>
@@ -5652,7 +5028,7 @@
       <c r="AB111" s="13"/>
       <c r="AC111" s="13"/>
     </row>
-    <row r="112" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="112" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
       <c r="C112" s="13"/>
@@ -5683,7 +5059,7 @@
       <c r="AB112" s="13"/>
       <c r="AC112" s="13"/>
     </row>
-    <row r="113" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="113" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A113" s="13"/>
       <c r="B113" s="13"/>
       <c r="C113" s="13"/>
@@ -5714,7 +5090,7 @@
       <c r="AB113" s="13"/>
       <c r="AC113" s="13"/>
     </row>
-    <row r="114" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="114" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A114" s="13"/>
       <c r="B114" s="13"/>
       <c r="C114" s="13"/>
@@ -5745,7 +5121,7 @@
       <c r="AB114" s="13"/>
       <c r="AC114" s="13"/>
     </row>
-    <row r="115" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="115" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A115" s="13"/>
       <c r="B115" s="13"/>
       <c r="C115" s="13"/>
@@ -5776,7 +5152,7 @@
       <c r="AB115" s="13"/>
       <c r="AC115" s="13"/>
     </row>
-    <row r="116" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="116" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A116" s="13"/>
       <c r="B116" s="13"/>
       <c r="C116" s="13"/>
@@ -5807,7 +5183,7 @@
       <c r="AB116" s="13"/>
       <c r="AC116" s="13"/>
     </row>
-    <row r="117" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="117" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A117" s="13"/>
       <c r="B117" s="13"/>
       <c r="C117" s="13"/>
@@ -5838,7 +5214,7 @@
       <c r="AB117" s="13"/>
       <c r="AC117" s="13"/>
     </row>
-    <row r="118" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="118" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A118" s="13"/>
       <c r="B118" s="13"/>
       <c r="C118" s="13"/>
@@ -5869,7 +5245,7 @@
       <c r="AB118" s="13"/>
       <c r="AC118" s="13"/>
     </row>
-    <row r="119" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="119" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A119" s="13"/>
       <c r="B119" s="13"/>
       <c r="C119" s="13"/>
@@ -5900,7 +5276,7 @@
       <c r="AB119" s="13"/>
       <c r="AC119" s="13"/>
     </row>
-    <row r="120" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="120" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A120" s="13"/>
       <c r="B120" s="13"/>
       <c r="C120" s="13"/>
@@ -5931,7 +5307,7 @@
       <c r="AB120" s="13"/>
       <c r="AC120" s="13"/>
     </row>
-    <row r="121" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="121" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A121" s="13"/>
       <c r="B121" s="13"/>
       <c r="C121" s="13"/>
@@ -5962,7 +5338,7 @@
       <c r="AB121" s="13"/>
       <c r="AC121" s="13"/>
     </row>
-    <row r="122" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="122" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A122" s="13"/>
       <c r="B122" s="13"/>
       <c r="C122" s="13"/>
@@ -5993,7 +5369,7 @@
       <c r="AB122" s="13"/>
       <c r="AC122" s="13"/>
     </row>
-    <row r="123" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="123" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A123" s="13"/>
       <c r="B123" s="13"/>
       <c r="C123" s="13"/>
@@ -6024,7 +5400,7 @@
       <c r="AB123" s="13"/>
       <c r="AC123" s="13"/>
     </row>
-    <row r="124" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="124" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A124" s="13"/>
       <c r="B124" s="13"/>
       <c r="C124" s="13"/>
@@ -6055,7 +5431,7 @@
       <c r="AB124" s="13"/>
       <c r="AC124" s="13"/>
     </row>
-    <row r="125" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="125" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A125" s="13"/>
       <c r="B125" s="13"/>
       <c r="C125" s="13"/>
@@ -6086,7 +5462,7 @@
       <c r="AB125" s="13"/>
       <c r="AC125" s="13"/>
     </row>
-    <row r="126" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="126" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A126" s="13"/>
       <c r="B126" s="13"/>
       <c r="C126" s="13"/>
@@ -6117,7 +5493,7 @@
       <c r="AB126" s="13"/>
       <c r="AC126" s="13"/>
     </row>
-    <row r="127" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="127" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A127" s="13"/>
       <c r="B127" s="13"/>
       <c r="C127" s="13"/>
@@ -6148,7 +5524,7 @@
       <c r="AB127" s="13"/>
       <c r="AC127" s="13"/>
     </row>
-    <row r="128" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="128" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A128" s="13"/>
       <c r="B128" s="13"/>
       <c r="C128" s="13"/>
@@ -6179,7 +5555,7 @@
       <c r="AB128" s="13"/>
       <c r="AC128" s="13"/>
     </row>
-    <row r="129" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="129" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A129" s="13"/>
       <c r="B129" s="13"/>
       <c r="C129" s="13"/>
@@ -6210,7 +5586,7 @@
       <c r="AB129" s="13"/>
       <c r="AC129" s="13"/>
     </row>
-    <row r="130" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="130" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A130" s="13"/>
       <c r="B130" s="13"/>
       <c r="C130" s="13"/>
@@ -6241,7 +5617,7 @@
       <c r="AB130" s="13"/>
       <c r="AC130" s="13"/>
     </row>
-    <row r="131" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="131" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A131" s="13"/>
       <c r="B131" s="13"/>
       <c r="C131" s="13"/>
@@ -6272,7 +5648,7 @@
       <c r="AB131" s="13"/>
       <c r="AC131" s="13"/>
     </row>
-    <row r="132" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="132" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A132" s="13"/>
       <c r="B132" s="13"/>
       <c r="C132" s="13"/>
@@ -6303,7 +5679,7 @@
       <c r="AB132" s="13"/>
       <c r="AC132" s="13"/>
     </row>
-    <row r="133" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="133" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A133" s="13"/>
       <c r="B133" s="13"/>
       <c r="C133" s="13"/>
@@ -6334,7 +5710,7 @@
       <c r="AB133" s="13"/>
       <c r="AC133" s="13"/>
     </row>
-    <row r="134" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="134" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A134" s="13"/>
       <c r="B134" s="13"/>
       <c r="C134" s="13"/>
@@ -6365,7 +5741,7 @@
       <c r="AB134" s="13"/>
       <c r="AC134" s="13"/>
     </row>
-    <row r="135" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="135" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A135" s="13"/>
       <c r="B135" s="13"/>
       <c r="C135" s="13"/>
@@ -6396,7 +5772,7 @@
       <c r="AB135" s="13"/>
       <c r="AC135" s="13"/>
     </row>
-    <row r="136" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="136" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A136" s="13"/>
       <c r="B136" s="13"/>
       <c r="C136" s="13"/>
@@ -6427,7 +5803,7 @@
       <c r="AB136" s="13"/>
       <c r="AC136" s="13"/>
     </row>
-    <row r="137" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="137" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A137" s="13"/>
       <c r="B137" s="13"/>
       <c r="C137" s="13"/>
@@ -6458,7 +5834,7 @@
       <c r="AB137" s="13"/>
       <c r="AC137" s="13"/>
     </row>
-    <row r="138" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="138" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A138" s="13"/>
       <c r="B138" s="13"/>
       <c r="C138" s="13"/>
@@ -6489,7 +5865,7 @@
       <c r="AB138" s="13"/>
       <c r="AC138" s="13"/>
     </row>
-    <row r="139" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="139" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A139" s="13"/>
       <c r="B139" s="13"/>
       <c r="C139" s="13"/>
@@ -6520,7 +5896,7 @@
       <c r="AB139" s="13"/>
       <c r="AC139" s="13"/>
     </row>
-    <row r="140" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="140" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A140" s="13"/>
       <c r="B140" s="13"/>
       <c r="C140" s="13"/>
@@ -6551,7 +5927,7 @@
       <c r="AB140" s="13"/>
       <c r="AC140" s="13"/>
     </row>
-    <row r="141" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="141" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A141" s="13"/>
       <c r="B141" s="13"/>
       <c r="C141" s="13"/>
@@ -6582,7 +5958,7 @@
       <c r="AB141" s="13"/>
       <c r="AC141" s="13"/>
     </row>
-    <row r="142" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="142" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A142" s="13"/>
       <c r="B142" s="13"/>
       <c r="C142" s="13"/>
@@ -6613,7 +5989,7 @@
       <c r="AB142" s="13"/>
       <c r="AC142" s="13"/>
     </row>
-    <row r="143" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="143" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A143" s="13"/>
       <c r="B143" s="13"/>
       <c r="C143" s="13"/>
@@ -6644,7 +6020,7 @@
       <c r="AB143" s="13"/>
       <c r="AC143" s="13"/>
     </row>
-    <row r="144" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="144" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A144" s="13"/>
       <c r="B144" s="13"/>
       <c r="C144" s="13"/>
@@ -6675,7 +6051,7 @@
       <c r="AB144" s="13"/>
       <c r="AC144" s="13"/>
     </row>
-    <row r="145" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="145" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A145" s="13"/>
       <c r="B145" s="13"/>
       <c r="C145" s="13"/>
@@ -6706,7 +6082,7 @@
       <c r="AB145" s="13"/>
       <c r="AC145" s="13"/>
     </row>
-    <row r="146" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="146" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A146" s="13"/>
       <c r="B146" s="13"/>
       <c r="C146" s="13"/>
@@ -6737,7 +6113,7 @@
       <c r="AB146" s="13"/>
       <c r="AC146" s="13"/>
     </row>
-    <row r="147" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="147" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A147" s="13"/>
       <c r="B147" s="13"/>
       <c r="C147" s="13"/>
@@ -6768,7 +6144,7 @@
       <c r="AB147" s="13"/>
       <c r="AC147" s="13"/>
     </row>
-    <row r="148" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="148" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A148" s="13"/>
       <c r="B148" s="13"/>
       <c r="C148" s="13"/>
@@ -6799,7 +6175,7 @@
       <c r="AB148" s="13"/>
       <c r="AC148" s="13"/>
     </row>
-    <row r="149" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="149" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A149" s="13"/>
       <c r="B149" s="13"/>
       <c r="C149" s="13"/>
@@ -6830,7 +6206,7 @@
       <c r="AB149" s="13"/>
       <c r="AC149" s="13"/>
     </row>
-    <row r="150" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="150" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A150" s="13"/>
       <c r="B150" s="13"/>
       <c r="C150" s="13"/>
@@ -6861,7 +6237,7 @@
       <c r="AB150" s="13"/>
       <c r="AC150" s="13"/>
     </row>
-    <row r="151" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="151" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A151" s="13"/>
       <c r="B151" s="13"/>
       <c r="C151" s="13"/>
@@ -6892,7 +6268,7 @@
       <c r="AB151" s="13"/>
       <c r="AC151" s="13"/>
     </row>
-    <row r="152" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="152" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A152" s="13"/>
       <c r="B152" s="13"/>
       <c r="C152" s="13"/>
@@ -6923,7 +6299,7 @@
       <c r="AB152" s="13"/>
       <c r="AC152" s="13"/>
     </row>
-    <row r="153" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="153" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A153" s="13"/>
       <c r="B153" s="13"/>
       <c r="C153" s="13"/>
@@ -6954,7 +6330,7 @@
       <c r="AB153" s="13"/>
       <c r="AC153" s="13"/>
     </row>
-    <row r="154" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="154" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A154" s="13"/>
       <c r="B154" s="13"/>
       <c r="C154" s="13"/>
@@ -6985,7 +6361,7 @@
       <c r="AB154" s="13"/>
       <c r="AC154" s="13"/>
     </row>
-    <row r="155" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="155" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A155" s="13"/>
       <c r="B155" s="13"/>
       <c r="C155" s="13"/>
@@ -7016,7 +6392,7 @@
       <c r="AB155" s="13"/>
       <c r="AC155" s="13"/>
     </row>
-    <row r="156" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="156" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A156" s="13"/>
       <c r="B156" s="13"/>
       <c r="C156" s="13"/>
@@ -7047,7 +6423,7 @@
       <c r="AB156" s="13"/>
       <c r="AC156" s="13"/>
     </row>
-    <row r="157" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="157" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A157" s="13"/>
       <c r="B157" s="13"/>
       <c r="C157" s="13"/>
@@ -7078,7 +6454,7 @@
       <c r="AB157" s="13"/>
       <c r="AC157" s="13"/>
     </row>
-    <row r="158" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="158" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A158" s="13"/>
       <c r="B158" s="13"/>
       <c r="C158" s="13"/>
@@ -7109,7 +6485,7 @@
       <c r="AB158" s="13"/>
       <c r="AC158" s="13"/>
     </row>
-    <row r="159" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="159" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A159" s="13"/>
       <c r="B159" s="13"/>
       <c r="C159" s="13"/>
@@ -7140,7 +6516,7 @@
       <c r="AB159" s="13"/>
       <c r="AC159" s="13"/>
     </row>
-    <row r="160" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="160" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A160" s="13"/>
       <c r="B160" s="13"/>
       <c r="C160" s="13"/>
@@ -7171,7 +6547,7 @@
       <c r="AB160" s="13"/>
       <c r="AC160" s="13"/>
     </row>
-    <row r="161" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="161" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A161" s="13"/>
       <c r="B161" s="13"/>
       <c r="C161" s="13"/>
@@ -7202,7 +6578,7 @@
       <c r="AB161" s="13"/>
       <c r="AC161" s="13"/>
     </row>
-    <row r="162" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="162" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A162" s="13"/>
       <c r="B162" s="13"/>
       <c r="C162" s="13"/>
@@ -7233,7 +6609,7 @@
       <c r="AB162" s="13"/>
       <c r="AC162" s="13"/>
     </row>
-    <row r="163" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="163" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A163" s="13"/>
       <c r="B163" s="13"/>
       <c r="C163" s="13"/>
@@ -7264,7 +6640,7 @@
       <c r="AB163" s="13"/>
       <c r="AC163" s="13"/>
     </row>
-    <row r="164" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="164" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A164" s="13"/>
       <c r="B164" s="13"/>
       <c r="C164" s="13"/>
@@ -7295,7 +6671,7 @@
       <c r="AB164" s="13"/>
       <c r="AC164" s="13"/>
     </row>
-    <row r="165" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="165" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A165" s="13"/>
       <c r="B165" s="13"/>
       <c r="C165" s="13"/>
@@ -7326,7 +6702,7 @@
       <c r="AB165" s="13"/>
       <c r="AC165" s="13"/>
     </row>
-    <row r="166" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="166" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A166" s="13"/>
       <c r="B166" s="13"/>
       <c r="C166" s="13"/>
@@ -7357,7 +6733,7 @@
       <c r="AB166" s="13"/>
       <c r="AC166" s="13"/>
     </row>
-    <row r="167" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="167" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A167" s="13"/>
       <c r="B167" s="13"/>
       <c r="C167" s="13"/>
@@ -7388,7 +6764,7 @@
       <c r="AB167" s="13"/>
       <c r="AC167" s="13"/>
     </row>
-    <row r="168" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="168" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A168" s="13"/>
       <c r="B168" s="13"/>
       <c r="C168" s="13"/>
@@ -7419,7 +6795,7 @@
       <c r="AB168" s="13"/>
       <c r="AC168" s="13"/>
     </row>
-    <row r="169" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="169" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A169" s="13"/>
       <c r="B169" s="13"/>
       <c r="C169" s="13"/>
@@ -7450,7 +6826,7 @@
       <c r="AB169" s="13"/>
       <c r="AC169" s="13"/>
     </row>
-    <row r="170" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="170" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A170" s="13"/>
       <c r="B170" s="13"/>
       <c r="C170" s="13"/>
@@ -7481,7 +6857,7 @@
       <c r="AB170" s="13"/>
       <c r="AC170" s="13"/>
     </row>
-    <row r="171" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="171" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A171" s="13"/>
       <c r="B171" s="13"/>
       <c r="C171" s="13"/>
@@ -7512,7 +6888,7 @@
       <c r="AB171" s="13"/>
       <c r="AC171" s="13"/>
     </row>
-    <row r="172" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="172" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A172" s="13"/>
       <c r="B172" s="13"/>
       <c r="C172" s="13"/>
@@ -7543,7 +6919,7 @@
       <c r="AB172" s="13"/>
       <c r="AC172" s="13"/>
     </row>
-    <row r="173" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="173" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A173" s="13"/>
       <c r="B173" s="13"/>
       <c r="C173" s="13"/>
@@ -7574,7 +6950,7 @@
       <c r="AB173" s="13"/>
       <c r="AC173" s="13"/>
     </row>
-    <row r="174" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="174" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A174" s="13"/>
       <c r="B174" s="13"/>
       <c r="C174" s="13"/>
@@ -7605,7 +6981,7 @@
       <c r="AB174" s="13"/>
       <c r="AC174" s="13"/>
     </row>
-    <row r="175" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="175" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A175" s="13"/>
       <c r="B175" s="13"/>
       <c r="C175" s="13"/>
@@ -7636,7 +7012,7 @@
       <c r="AB175" s="13"/>
       <c r="AC175" s="13"/>
     </row>
-    <row r="176" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="176" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A176" s="13"/>
       <c r="B176" s="13"/>
       <c r="C176" s="13"/>
@@ -7667,7 +7043,7 @@
       <c r="AB176" s="13"/>
       <c r="AC176" s="13"/>
     </row>
-    <row r="177" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="177" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A177" s="13"/>
       <c r="B177" s="13"/>
       <c r="C177" s="13"/>
@@ -7698,7 +7074,7 @@
       <c r="AB177" s="13"/>
       <c r="AC177" s="13"/>
     </row>
-    <row r="178" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="178" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A178" s="13"/>
       <c r="B178" s="13"/>
       <c r="C178" s="13"/>
@@ -7729,7 +7105,7 @@
       <c r="AB178" s="13"/>
       <c r="AC178" s="13"/>
     </row>
-    <row r="179" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="179" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A179" s="13"/>
       <c r="B179" s="13"/>
       <c r="C179" s="13"/>
@@ -7760,7 +7136,7 @@
       <c r="AB179" s="13"/>
       <c r="AC179" s="13"/>
     </row>
-    <row r="180" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="180" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A180" s="13"/>
       <c r="B180" s="13"/>
       <c r="C180" s="13"/>
@@ -7791,7 +7167,7 @@
       <c r="AB180" s="13"/>
       <c r="AC180" s="13"/>
     </row>
-    <row r="181" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="181" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A181" s="13"/>
       <c r="B181" s="13"/>
       <c r="C181" s="13"/>
@@ -7822,7 +7198,7 @@
       <c r="AB181" s="13"/>
       <c r="AC181" s="13"/>
     </row>
-    <row r="182" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="182" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A182" s="13"/>
       <c r="B182" s="13"/>
       <c r="C182" s="13"/>
@@ -7853,7 +7229,7 @@
       <c r="AB182" s="13"/>
       <c r="AC182" s="13"/>
     </row>
-    <row r="183" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="183" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A183" s="13"/>
       <c r="B183" s="13"/>
       <c r="C183" s="13"/>
@@ -7884,7 +7260,7 @@
       <c r="AB183" s="13"/>
       <c r="AC183" s="13"/>
     </row>
-    <row r="184" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="184" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A184" s="13"/>
       <c r="B184" s="13"/>
       <c r="C184" s="13"/>
@@ -7915,7 +7291,7 @@
       <c r="AB184" s="13"/>
       <c r="AC184" s="13"/>
     </row>
-    <row r="185" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="185" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A185" s="13"/>
       <c r="B185" s="13"/>
       <c r="C185" s="13"/>
@@ -7946,7 +7322,7 @@
       <c r="AB185" s="13"/>
       <c r="AC185" s="13"/>
     </row>
-    <row r="186" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="186" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A186" s="13"/>
       <c r="B186" s="13"/>
       <c r="C186" s="13"/>
@@ -7977,7 +7353,7 @@
       <c r="AB186" s="13"/>
       <c r="AC186" s="13"/>
     </row>
-    <row r="187" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="187" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A187" s="13"/>
       <c r="B187" s="13"/>
       <c r="C187" s="13"/>
@@ -8008,7 +7384,7 @@
       <c r="AB187" s="13"/>
       <c r="AC187" s="13"/>
     </row>
-    <row r="188" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="188" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A188" s="13"/>
       <c r="B188" s="13"/>
       <c r="C188" s="13"/>
@@ -8039,7 +7415,7 @@
       <c r="AB188" s="13"/>
       <c r="AC188" s="13"/>
     </row>
-    <row r="189" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="189" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A189" s="13"/>
       <c r="B189" s="13"/>
       <c r="C189" s="13"/>
@@ -8070,7 +7446,7 @@
       <c r="AB189" s="13"/>
       <c r="AC189" s="13"/>
     </row>
-    <row r="190" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="190" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A190" s="13"/>
       <c r="B190" s="13"/>
       <c r="C190" s="13"/>
@@ -8101,7 +7477,7 @@
       <c r="AB190" s="13"/>
       <c r="AC190" s="13"/>
     </row>
-    <row r="191" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="191" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A191" s="13"/>
       <c r="B191" s="13"/>
       <c r="C191" s="13"/>
@@ -8132,7 +7508,7 @@
       <c r="AB191" s="13"/>
       <c r="AC191" s="13"/>
     </row>
-    <row r="192" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="192" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A192" s="13"/>
       <c r="B192" s="13"/>
       <c r="C192" s="13"/>
@@ -8163,7 +7539,7 @@
       <c r="AB192" s="13"/>
       <c r="AC192" s="13"/>
     </row>
-    <row r="193" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="193" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A193" s="13"/>
       <c r="B193" s="13"/>
       <c r="C193" s="13"/>
@@ -8194,7 +7570,7 @@
       <c r="AB193" s="13"/>
       <c r="AC193" s="13"/>
     </row>
-    <row r="194" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="194" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A194" s="13"/>
       <c r="B194" s="13"/>
       <c r="C194" s="13"/>
@@ -8225,7 +7601,7 @@
       <c r="AB194" s="13"/>
       <c r="AC194" s="13"/>
     </row>
-    <row r="195" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="195" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A195" s="13"/>
       <c r="B195" s="13"/>
       <c r="C195" s="13"/>
@@ -8256,7 +7632,7 @@
       <c r="AB195" s="13"/>
       <c r="AC195" s="13"/>
     </row>
-    <row r="196" s="3" customFormat="1" ht="16" customHeight="1" spans="1:29">
+    <row r="196" spans="1:29" s="3" customFormat="1" ht="16" customHeight="1">
       <c r="A196" s="13"/>
       <c r="B196" s="13"/>
       <c r="C196" s="13"/>
@@ -8289,18 +7665,18 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N196">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N196" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"妈妈,爸爸,奶奶,爷爷,外婆,外公,其他"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B196">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B196" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"待产期,已出生"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D196">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D196" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"男,女,未知"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>